<commit_message>
fixing BU calculating and average per BU
</commit_message>
<xml_diff>
--- a/data/filterSuporteMilho.xlsx
+++ b/data/filterSuporteMilho.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christiano/Documents/analysis/reporteSemanal/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syngenta-my.sharepoint.com/personal/chris_simoes_syngenta_com/Documents/Documents/AnalysisR/reporteSemanal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD138EF3-945C-EE4C-9381-0505CE0DB7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{CD138EF3-945C-EE4C-9381-0505CE0DB7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7173DED-3ADA-4A44-847D-FE05718EC84B}"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="500" windowWidth="22060" windowHeight="16420" xr2:uid="{D3691A72-1D75-4D53-A4B7-90B12D9BB150}"/>
+    <workbookView xWindow="12000" yWindow="2040" windowWidth="19110" windowHeight="13635" xr2:uid="{D3691A72-1D75-4D53-A4B7-90B12D9BB150}"/>
   </bookViews>
   <sheets>
     <sheet name="Checks" sheetId="26" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sinonimos" sheetId="28" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Checks!$A$1:$I$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Checks!$A$1:$I$119</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sinonimos!$A$1:$B$124</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="263">
   <si>
     <t>Check</t>
   </si>
@@ -835,7 +835,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -888,6 +888,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -909,7 +917,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -977,6 +985,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -995,7 +1006,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1292,25 +1303,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EDAA8D-8E1B-4C97-952E-CACA70ECA49E}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:W121"/>
+  <dimension ref="A1:W120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:I18"/>
+      <selection activeCell="H120" sqref="H120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="20" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="8.5" style="18" customWidth="1"/>
-    <col min="7" max="9" width="9.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="13"/>
+    <col min="1" max="1" width="14.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="18" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
@@ -1339,7 +1350,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>19</v>
       </c>
@@ -1368,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>254</v>
       </c>
@@ -1397,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>254</v>
       </c>
@@ -1426,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>154</v>
       </c>
@@ -1455,7 +1466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>154</v>
       </c>
@@ -1478,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>21</v>
       </c>
@@ -1507,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>21</v>
       </c>
@@ -1536,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>31</v>
       </c>
@@ -1565,7 +1576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>70</v>
       </c>
@@ -1594,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>29</v>
       </c>
@@ -1623,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>57</v>
       </c>
@@ -1652,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>17</v>
       </c>
@@ -1681,7 +1692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>17</v>
       </c>
@@ -1710,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
@@ -1739,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
@@ -1768,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>39</v>
       </c>
@@ -1791,13 +1802,13 @@
         <v>0</v>
       </c>
       <c r="H17" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>18</v>
       </c>
@@ -1826,7 +1837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>253</v>
       </c>
@@ -1849,13 +1860,13 @@
         <v>1</v>
       </c>
       <c r="H19" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>253</v>
       </c>
@@ -1884,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>253</v>
       </c>
@@ -1913,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>253</v>
       </c>
@@ -1942,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>253</v>
       </c>
@@ -1971,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>253</v>
       </c>
@@ -2000,7 +2011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>253</v>
       </c>
@@ -2029,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>253</v>
       </c>
@@ -2058,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>252</v>
       </c>
@@ -2087,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>252</v>
       </c>
@@ -2116,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>36</v>
       </c>
@@ -2139,13 +2150,13 @@
         <v>1</v>
       </c>
       <c r="H29" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>251</v>
       </c>
@@ -2174,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>251</v>
       </c>
@@ -2203,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>106</v>
       </c>
@@ -2232,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>106</v>
       </c>
@@ -2261,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>106</v>
       </c>
@@ -2290,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>16</v>
       </c>
@@ -2319,7 +2330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>16</v>
       </c>
@@ -2348,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>16</v>
       </c>
@@ -2377,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>33</v>
       </c>
@@ -2406,7 +2417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>33</v>
       </c>
@@ -2435,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>22</v>
       </c>
@@ -2464,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>66</v>
       </c>
@@ -2493,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>32</v>
       </c>
@@ -2522,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>32</v>
       </c>
@@ -2551,7 +2562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>128</v>
       </c>
@@ -2580,7 +2591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>128</v>
       </c>
@@ -2609,7 +2620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>128</v>
       </c>
@@ -2638,7 +2649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>128</v>
       </c>
@@ -2667,7 +2678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>107</v>
       </c>
@@ -2696,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
         <v>107</v>
       </c>
@@ -2725,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>250</v>
       </c>
@@ -2754,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>107</v>
       </c>
@@ -2783,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>35</v>
       </c>
@@ -2817,7 +2828,7 @@
       <c r="S52" s="10"/>
       <c r="T52" s="9"/>
     </row>
-    <row r="53" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>37</v>
       </c>
@@ -2853,7 +2864,7 @@
       <c r="V53" s="9"/>
       <c r="W53" s="9"/>
     </row>
-    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
         <v>37</v>
       </c>
@@ -2882,7 +2893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>27</v>
       </c>
@@ -2911,7 +2922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
         <v>27</v>
       </c>
@@ -2940,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
         <v>48</v>
       </c>
@@ -2969,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
         <v>34</v>
       </c>
@@ -2998,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
         <v>34</v>
       </c>
@@ -3027,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>111</v>
       </c>
@@ -3056,7 +3067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
         <v>111</v>
       </c>
@@ -3085,7 +3096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
         <v>112</v>
       </c>
@@ -3114,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
         <v>112</v>
       </c>
@@ -3143,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>114</v>
       </c>
@@ -3172,7 +3183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
         <v>131</v>
       </c>
@@ -3201,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
         <v>121</v>
       </c>
@@ -3230,7 +3241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
         <v>127</v>
       </c>
@@ -3259,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
         <v>127</v>
       </c>
@@ -3288,7 +3299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
         <v>127</v>
       </c>
@@ -3317,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
         <v>127</v>
       </c>
@@ -3346,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
         <v>127</v>
       </c>
@@ -3375,9 +3386,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="B72" s="12">
         <v>1</v>
@@ -3386,10 +3397,10 @@
         <v>10</v>
       </c>
       <c r="D72" s="20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" s="18">
         <v>1</v>
@@ -3404,9 +3415,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="B73" s="12">
         <v>1</v>
@@ -3415,13 +3426,16 @@
         <v>10</v>
       </c>
       <c r="D73" s="20">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="E73" s="18" t="s">
+        <v>6</v>
       </c>
       <c r="F73" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73" s="18">
         <v>0</v>
@@ -3430,27 +3444,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="B74" s="12">
+        <v>153</v>
+      </c>
+      <c r="B74" s="18">
         <v>1</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D74" s="20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F74" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" s="18">
         <v>0</v>
@@ -3459,18 +3473,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B75" s="12">
+        <v>153</v>
+      </c>
+      <c r="B75" s="18">
         <v>1</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D75" s="20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E75" s="18" t="s">
         <v>6</v>
@@ -3488,94 +3502,94 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="B76" s="18">
-        <v>1</v>
-      </c>
-      <c r="C76" s="18" t="s">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B76" s="23">
+        <v>1</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="D76" s="25">
+        <v>7</v>
+      </c>
+      <c r="E76" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" s="18">
+        <v>1</v>
+      </c>
+      <c r="G76" s="18">
+        <v>0</v>
+      </c>
+      <c r="H76" s="18">
+        <v>0</v>
+      </c>
+      <c r="I76" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B77" s="12">
+        <v>1</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" s="20">
+        <v>5</v>
+      </c>
+      <c r="E77" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77" s="18">
+        <v>0</v>
+      </c>
+      <c r="G77" s="18">
+        <v>1</v>
+      </c>
+      <c r="H77" s="18">
+        <v>0</v>
+      </c>
+      <c r="I77" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B78" s="18">
+        <v>1</v>
+      </c>
+      <c r="C78" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D76" s="20">
-        <v>7</v>
-      </c>
-      <c r="E76" s="18" t="s">
+      <c r="D78" s="20">
+        <v>7</v>
+      </c>
+      <c r="E78" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F76" s="18">
-        <v>0</v>
-      </c>
-      <c r="G76" s="18">
-        <v>0</v>
-      </c>
-      <c r="H76" s="18">
-        <v>0</v>
-      </c>
-      <c r="I76" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="B77" s="18">
-        <v>1</v>
-      </c>
-      <c r="C77" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" s="20">
-        <v>3</v>
-      </c>
-      <c r="E77" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F77" s="18">
-        <v>0</v>
-      </c>
-      <c r="G77" s="18">
-        <v>0</v>
-      </c>
-      <c r="H77" s="18">
-        <v>0</v>
-      </c>
-      <c r="I77" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B78" s="23">
-        <v>1</v>
-      </c>
-      <c r="C78" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="D78" s="25">
-        <v>7</v>
-      </c>
-      <c r="E78" s="23" t="s">
-        <v>8</v>
-      </c>
       <c r="F78" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H78" s="18">
         <v>0</v>
       </c>
       <c r="I78" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
         <v>115</v>
       </c>
@@ -3583,48 +3597,48 @@
         <v>1</v>
       </c>
       <c r="C79" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79" s="20">
+        <v>4</v>
+      </c>
+      <c r="E79" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F79" s="18">
+        <v>0</v>
+      </c>
+      <c r="G79" s="18">
+        <v>1</v>
+      </c>
+      <c r="H79" s="18">
+        <v>0</v>
+      </c>
+      <c r="I79" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B80" s="12">
+        <v>1</v>
+      </c>
+      <c r="C80" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D79" s="20">
-        <v>5</v>
-      </c>
-      <c r="E79" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F79" s="18">
-        <v>0</v>
-      </c>
-      <c r="G79" s="18">
-        <v>1</v>
-      </c>
-      <c r="H79" s="18">
-        <v>0</v>
-      </c>
-      <c r="I79" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="B80" s="18">
-        <v>1</v>
-      </c>
-      <c r="C80" s="18" t="s">
-        <v>11</v>
-      </c>
       <c r="D80" s="20">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F80" s="18">
         <v>0</v>
       </c>
       <c r="G80" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H80" s="18">
         <v>0</v>
@@ -3633,18 +3647,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B81" s="12">
         <v>1</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D81" s="20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E81" s="18" t="s">
         <v>6</v>
@@ -3653,7 +3667,7 @@
         <v>0</v>
       </c>
       <c r="G81" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" s="18">
         <v>0</v>
@@ -3662,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
         <v>123</v>
       </c>
@@ -3670,13 +3684,13 @@
         <v>1</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D82" s="20">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="D82" s="18">
+        <v>5</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F82" s="18">
         <v>0</v>
@@ -3691,7 +3705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
         <v>123</v>
       </c>
@@ -3699,13 +3713,13 @@
         <v>1</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D83" s="20">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="D83" s="18">
+        <v>5</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F83" s="18">
         <v>0</v>
@@ -3720,7 +3734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
         <v>123</v>
       </c>
@@ -3728,7 +3742,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D84" s="18">
         <v>5</v>
@@ -3749,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
         <v>123</v>
       </c>
@@ -3757,7 +3771,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D85" s="18">
         <v>5</v>
@@ -3778,7 +3792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
         <v>123</v>
       </c>
@@ -3786,13 +3800,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D86" s="18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E86" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" s="18">
         <v>0</v>
@@ -3807,7 +3821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="18" t="s">
         <v>123</v>
       </c>
@@ -3815,71 +3829,71 @@
         <v>1</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D87" s="18">
+        <v>4</v>
+      </c>
+      <c r="E87" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F87" s="18">
+        <v>0</v>
+      </c>
+      <c r="G87" s="18">
+        <v>0</v>
+      </c>
+      <c r="H87" s="18">
+        <v>0</v>
+      </c>
+      <c r="I87" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B88" s="18">
+        <v>1</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="20">
+        <v>7</v>
+      </c>
+      <c r="E88" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88" s="18">
+        <v>0</v>
+      </c>
+      <c r="G88" s="18">
+        <v>0</v>
+      </c>
+      <c r="H88" s="18">
+        <v>0</v>
+      </c>
+      <c r="I88" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B89" s="12">
+        <v>1</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D89" s="20">
         <v>5</v>
       </c>
-      <c r="E87" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F87" s="18">
-        <v>0</v>
-      </c>
-      <c r="G87" s="18">
-        <v>0</v>
-      </c>
-      <c r="H87" s="18">
-        <v>0</v>
-      </c>
-      <c r="I87" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B88" s="12">
-        <v>1</v>
-      </c>
-      <c r="C88" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D88" s="18">
-        <v>4</v>
-      </c>
-      <c r="E88" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F88" s="18">
-        <v>0</v>
-      </c>
-      <c r="G88" s="18">
-        <v>0</v>
-      </c>
-      <c r="H88" s="18">
-        <v>0</v>
-      </c>
-      <c r="I88" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B89" s="12">
-        <v>1</v>
-      </c>
-      <c r="C89" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D89" s="18">
-        <v>4</v>
-      </c>
       <c r="E89" s="18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F89" s="18">
         <v>0</v>
@@ -3891,41 +3905,41 @@
         <v>0</v>
       </c>
       <c r="I89" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B90" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B90" s="12">
         <v>1</v>
       </c>
       <c r="C90" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D90" s="20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E90" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F90" s="18">
         <v>0</v>
       </c>
       <c r="G90" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H90" s="18">
         <v>0</v>
       </c>
       <c r="I90" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="B91" s="12">
         <v>1</v>
@@ -3934,27 +3948,27 @@
         <v>10</v>
       </c>
       <c r="D91" s="20">
+        <v>2</v>
+      </c>
+      <c r="E91" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E91" s="18" t="s">
-        <v>7</v>
-      </c>
       <c r="F91" s="18">
         <v>0</v>
       </c>
       <c r="G91" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A92" s="22" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="B92" s="12">
         <v>1</v>
@@ -3963,11 +3977,11 @@
         <v>10</v>
       </c>
       <c r="D92" s="20">
+        <v>2</v>
+      </c>
+      <c r="E92" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E92" s="18" t="s">
-        <v>7</v>
-      </c>
       <c r="F92" s="18">
         <v>0</v>
       </c>
@@ -3975,21 +3989,21 @@
         <v>1</v>
       </c>
       <c r="H92" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I92" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B93" s="12">
+      <c r="B93" s="18">
         <v>1</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D93" s="20">
         <v>2</v>
@@ -4010,15 +4024,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="22" t="s">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B94" s="12">
+      <c r="B94" s="18">
         <v>1</v>
       </c>
       <c r="C94" s="18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D94" s="20">
         <v>2</v>
@@ -4039,15 +4053,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B95" s="18">
+      <c r="B95" s="12">
         <v>1</v>
       </c>
       <c r="C95" s="18" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D95" s="20">
         <v>2</v>
@@ -4068,38 +4082,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B96" s="18">
+        <v>88</v>
+      </c>
+      <c r="B96" s="12">
         <v>1</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D96" s="20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E96" s="18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F96" s="18">
         <v>0</v>
       </c>
       <c r="G96" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="18" t="s">
-        <v>139</v>
+        <v>28</v>
       </c>
       <c r="B97" s="12">
         <v>1</v>
@@ -4117,18 +4131,18 @@
         <v>0</v>
       </c>
       <c r="G97" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="18" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="B98" s="12">
         <v>1</v>
@@ -4155,154 +4169,154 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B99" s="12">
+        <v>20</v>
+      </c>
+      <c r="B99" s="18">
         <v>1</v>
       </c>
       <c r="C99" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D99" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E99" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F99" s="18">
+        <v>0</v>
+      </c>
+      <c r="G99" s="18">
+        <v>0</v>
+      </c>
+      <c r="H99" s="18">
+        <v>0</v>
+      </c>
+      <c r="I99" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B100" s="18">
+        <v>1</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="D100" s="20">
+        <v>6</v>
+      </c>
+      <c r="E100" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F100" s="18">
+        <v>0</v>
+      </c>
+      <c r="G100" s="18">
+        <v>0</v>
+      </c>
+      <c r="H100" s="18">
+        <v>0</v>
+      </c>
+      <c r="I100" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B101" s="18">
+        <v>1</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" s="20">
+        <v>7</v>
+      </c>
+      <c r="E101" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F101" s="18">
+        <v>1</v>
+      </c>
+      <c r="G101" s="18">
+        <v>1</v>
+      </c>
+      <c r="H101" s="18">
+        <v>1</v>
+      </c>
+      <c r="I101" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B102" s="12">
+        <v>1</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102" s="20">
         <v>5</v>
       </c>
-      <c r="F99" s="18">
-        <v>0</v>
-      </c>
-      <c r="G99" s="18">
-        <v>0</v>
-      </c>
-      <c r="H99" s="18">
-        <v>0</v>
-      </c>
-      <c r="I99" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B100" s="12">
-        <v>1</v>
-      </c>
-      <c r="C100" s="18" t="s">
+      <c r="E102" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F102" s="18">
+        <v>1</v>
+      </c>
+      <c r="G102" s="18">
+        <v>1</v>
+      </c>
+      <c r="H102" s="18">
+        <v>1</v>
+      </c>
+      <c r="I102" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B103" s="12">
+        <v>1</v>
+      </c>
+      <c r="C103" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D100" s="20">
-        <v>4</v>
-      </c>
-      <c r="E100" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F100" s="18">
-        <v>0</v>
-      </c>
-      <c r="G100" s="18">
-        <v>0</v>
-      </c>
-      <c r="H100" s="18">
-        <v>0</v>
-      </c>
-      <c r="I100" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B101" s="18">
-        <v>1</v>
-      </c>
-      <c r="C101" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D101" s="20">
+      <c r="D103" s="20">
         <v>5</v>
       </c>
-      <c r="E101" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F101" s="18">
-        <v>0</v>
-      </c>
-      <c r="G101" s="18">
-        <v>0</v>
-      </c>
-      <c r="H101" s="18">
-        <v>0</v>
-      </c>
-      <c r="I101" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="B102" s="18">
-        <v>1</v>
-      </c>
-      <c r="C102" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="D102" s="20">
-        <v>6</v>
-      </c>
-      <c r="E102" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F102" s="18">
-        <v>0</v>
-      </c>
-      <c r="G102" s="18">
-        <v>0</v>
-      </c>
-      <c r="H102" s="18">
-        <v>0</v>
-      </c>
-      <c r="I102" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B103" s="18">
-        <v>1</v>
-      </c>
-      <c r="C103" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D103" s="20">
-        <v>7</v>
-      </c>
       <c r="E103" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F103" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G103" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H103" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I103" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="22" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="18" t="s">
+        <v>108</v>
       </c>
       <c r="B104" s="12">
         <v>1</v>
@@ -4311,33 +4325,33 @@
         <v>10</v>
       </c>
       <c r="D104" s="20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E104" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F104" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G104" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H104" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I104" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A105" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B105" s="12">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B105" s="18">
         <v>1</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D105" s="20">
         <v>5</v>
@@ -4352,13 +4366,13 @@
         <v>0</v>
       </c>
       <c r="H105" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I105" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="18" t="s">
         <v>108</v>
       </c>
@@ -4366,7 +4380,7 @@
         <v>1</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D106" s="20">
         <v>4</v>
@@ -4387,53 +4401,53 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="B107" s="18">
+        <v>109</v>
+      </c>
+      <c r="B107" s="12">
         <v>1</v>
       </c>
       <c r="C107" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D107" s="20">
+        <v>4</v>
+      </c>
+      <c r="E107" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F107" s="18">
+        <v>1</v>
+      </c>
+      <c r="G107" s="18">
+        <v>0</v>
+      </c>
+      <c r="H107" s="18">
+        <v>0</v>
+      </c>
+      <c r="I107" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B108" s="18">
+        <v>1</v>
+      </c>
+      <c r="C108" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D107" s="20">
+      <c r="D108" s="20">
         <v>5</v>
       </c>
-      <c r="E107" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F107" s="18">
-        <v>0</v>
-      </c>
-      <c r="G107" s="18">
-        <v>0</v>
-      </c>
-      <c r="H107" s="18">
-        <v>0</v>
-      </c>
-      <c r="I107" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="B108" s="12">
-        <v>1</v>
-      </c>
-      <c r="C108" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D108" s="20">
-        <v>4</v>
-      </c>
       <c r="E108" s="18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F108" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G108" s="18">
         <v>0</v>
@@ -4442,10 +4456,10 @@
         <v>0</v>
       </c>
       <c r="I108" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
         <v>109</v>
       </c>
@@ -4453,13 +4467,13 @@
         <v>1</v>
       </c>
       <c r="C109" s="18" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D109" s="20">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E109" s="18" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F109" s="18">
         <v>1</v>
@@ -4474,15 +4488,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B110" s="18">
+        <v>257</v>
+      </c>
+      <c r="B110" s="12">
         <v>1</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D110" s="20">
         <v>5</v>
@@ -4491,7 +4505,7 @@
         <v>7</v>
       </c>
       <c r="F110" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G110" s="18">
         <v>0</v>
@@ -4500,18 +4514,18 @@
         <v>0</v>
       </c>
       <c r="I110" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="18" t="s">
-        <v>109</v>
+        <v>213</v>
       </c>
       <c r="B111" s="12">
         <v>1</v>
       </c>
       <c r="C111" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D111" s="20">
         <v>7</v>
@@ -4520,7 +4534,7 @@
         <v>8</v>
       </c>
       <c r="F111" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G111" s="18">
         <v>0</v>
@@ -4529,24 +4543,24 @@
         <v>0</v>
       </c>
       <c r="I111" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="B112" s="12">
+        <v>213</v>
+      </c>
+      <c r="B112" s="18">
         <v>1</v>
       </c>
       <c r="C112" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D112" s="20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E112" s="18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F112" s="18">
         <v>0</v>
@@ -4561,21 +4575,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="B113" s="12">
+      <c r="B113" s="18">
         <v>1</v>
       </c>
       <c r="C113" s="18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D113" s="20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E113" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F113" s="18">
         <v>0</v>
@@ -4590,15 +4604,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="B114" s="18">
+      <c r="B114" s="12">
         <v>1</v>
       </c>
       <c r="C114" s="18" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D114" s="20">
         <v>7</v>
@@ -4619,56 +4633,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="18" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="B115" s="18">
         <v>1</v>
       </c>
       <c r="C115" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115" s="20">
+        <v>7</v>
+      </c>
+      <c r="E115" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F115" s="18">
+        <v>1</v>
+      </c>
+      <c r="G115" s="18">
+        <v>1</v>
+      </c>
+      <c r="H115" s="18">
+        <v>0</v>
+      </c>
+      <c r="I115" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B116" s="18">
+        <v>1</v>
+      </c>
+      <c r="C116" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D115" s="20">
+      <c r="D116" s="20">
         <v>5</v>
       </c>
-      <c r="E115" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F115" s="18">
-        <v>0</v>
-      </c>
-      <c r="G115" s="18">
-        <v>0</v>
-      </c>
-      <c r="H115" s="18">
-        <v>0</v>
-      </c>
-      <c r="I115" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="B116" s="12">
-        <v>1</v>
-      </c>
-      <c r="C116" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D116" s="20">
-        <v>7</v>
-      </c>
       <c r="E116" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F116" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G116" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H116" s="18">
         <v>0</v>
@@ -4677,15 +4691,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="B117" s="18">
+        <v>255</v>
+      </c>
+      <c r="B117" s="12">
         <v>1</v>
       </c>
       <c r="C117" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D117" s="20">
         <v>7</v>
@@ -4694,27 +4708,27 @@
         <v>8</v>
       </c>
       <c r="F117" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G117" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H117" s="18">
         <v>0</v>
       </c>
       <c r="I117" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A118" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="B118" s="18">
+        <v>91</v>
+      </c>
+      <c r="B118" s="12">
         <v>1</v>
       </c>
       <c r="C118" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D118" s="20">
         <v>5</v>
@@ -4723,7 +4737,7 @@
         <v>7</v>
       </c>
       <c r="F118" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G118" s="18">
         <v>1</v>
@@ -4732,12 +4746,12 @@
         <v>0</v>
       </c>
       <c r="I118" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A119" s="18" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B119" s="12">
         <v>1</v>
@@ -4746,16 +4760,16 @@
         <v>10</v>
       </c>
       <c r="D119" s="20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E119" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F119" s="18">
         <v>0</v>
       </c>
       <c r="G119" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H119" s="18">
         <v>0</v>
@@ -4764,72 +4778,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B120" s="12">
-        <v>1</v>
-      </c>
-      <c r="C120" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D120" s="20">
-        <v>5</v>
-      </c>
-      <c r="E120" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F120" s="18">
-        <v>0</v>
-      </c>
-      <c r="G120" s="18">
-        <v>1</v>
-      </c>
-      <c r="H120" s="18">
-        <v>1</v>
-      </c>
-      <c r="I120" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="B121" s="12">
-        <v>1</v>
-      </c>
-      <c r="C121" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D121" s="20">
-        <v>5</v>
-      </c>
-      <c r="E121" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F121" s="18">
-        <v>0</v>
-      </c>
-      <c r="G121" s="18">
-        <v>1</v>
-      </c>
-      <c r="H121" s="18">
-        <v>1</v>
-      </c>
-      <c r="I121" s="18">
-        <v>0</v>
-      </c>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H120" s="27"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I121" xr:uid="{B0EDAA8D-8E1B-4C97-952E-CACA70ECA49E}">
+  <autoFilter ref="A1:I119" xr:uid="{B0EDAA8D-8E1B-4C97-952E-CACA70ECA49E}">
     <filterColumn colId="2">
       <filters>
         <filter val="COSTR"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I120">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I118">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -4847,13 +4811,13 @@
       <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -4861,7 +4825,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -4869,7 +4833,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
@@ -4877,7 +4841,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
@@ -4885,7 +4849,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -4893,7 +4857,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -4901,7 +4865,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -4909,7 +4873,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>67</v>
       </c>
@@ -4917,7 +4881,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>211</v>
       </c>
@@ -4939,13 +4903,13 @@
       <selection activeCell="A49" sqref="A49:B94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>248</v>
       </c>
@@ -4953,7 +4917,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -4961,7 +4925,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>230</v>
       </c>
@@ -4969,7 +4933,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>231</v>
       </c>
@@ -4977,7 +4941,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>79</v>
       </c>
@@ -4985,7 +4949,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>70</v>
       </c>
@@ -4993,7 +4957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>232</v>
       </c>
@@ -5001,7 +4965,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -5009,7 +4973,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>233</v>
       </c>
@@ -5017,7 +4981,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>234</v>
       </c>
@@ -5025,7 +4989,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>235</v>
       </c>
@@ -5033,7 +4997,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>156</v>
       </c>
@@ -5041,7 +5005,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>71</v>
       </c>
@@ -5049,7 +5013,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>158</v>
       </c>
@@ -5057,7 +5021,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>78</v>
       </c>
@@ -5065,7 +5029,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>85</v>
       </c>
@@ -5073,7 +5037,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>76</v>
       </c>
@@ -5081,7 +5045,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -5089,7 +5053,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>159</v>
       </c>
@@ -5097,7 +5061,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>160</v>
       </c>
@@ -5105,7 +5069,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -5113,7 +5077,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -5121,7 +5085,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>164</v>
       </c>
@@ -5129,7 +5093,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>165</v>
       </c>
@@ -5137,7 +5101,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>167</v>
       </c>
@@ -5145,7 +5109,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>168</v>
       </c>
@@ -5153,7 +5117,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>87</v>
       </c>
@@ -5161,7 +5125,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>83</v>
       </c>
@@ -5169,7 +5133,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
@@ -5177,7 +5141,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>75</v>
       </c>
@@ -5185,7 +5149,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>89</v>
       </c>
@@ -5193,7 +5157,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>84</v>
       </c>
@@ -5201,7 +5165,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>72</v>
       </c>
@@ -5209,7 +5173,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>77</v>
       </c>
@@ -5217,7 +5181,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>90</v>
       </c>
@@ -5225,7 +5189,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>88</v>
       </c>
@@ -5233,7 +5197,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>236</v>
       </c>
@@ -5241,7 +5205,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>82</v>
       </c>
@@ -5249,7 +5213,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -5257,7 +5221,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>169</v>
       </c>
@@ -5265,7 +5229,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>170</v>
       </c>
@@ -5273,7 +5237,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>171</v>
       </c>
@@ -5281,7 +5245,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>172</v>
       </c>
@@ -5289,7 +5253,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>173</v>
       </c>
@@ -5297,7 +5261,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>174</v>
       </c>
@@ -5305,7 +5269,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>175</v>
       </c>
@@ -5313,7 +5277,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -5321,7 +5285,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>177</v>
       </c>
@@ -5329,7 +5293,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>178</v>
       </c>
@@ -5337,7 +5301,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>242</v>
       </c>
@@ -5345,7 +5309,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -5353,7 +5317,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>43</v>
       </c>
@@ -5361,7 +5325,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>224</v>
       </c>
@@ -5369,7 +5333,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>224</v>
       </c>
@@ -5377,7 +5341,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>214</v>
       </c>
@@ -5385,7 +5349,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>225</v>
       </c>
@@ -5393,7 +5357,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>227</v>
       </c>
@@ -5401,7 +5365,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>226</v>
       </c>
@@ -5409,7 +5373,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>44</v>
       </c>
@@ -5417,7 +5381,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>229</v>
       </c>
@@ -5425,7 +5389,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>229</v>
       </c>
@@ -5433,7 +5397,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>45</v>
       </c>
@@ -5441,7 +5405,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>217</v>
       </c>
@@ -5449,7 +5413,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>40</v>
       </c>
@@ -5457,7 +5421,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>219</v>
       </c>
@@ -5465,7 +5429,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>228</v>
       </c>
@@ -5473,7 +5437,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>215</v>
       </c>
@@ -5481,7 +5445,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>179</v>
       </c>
@@ -5489,7 +5453,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>180</v>
       </c>
@@ -5497,7 +5461,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>181</v>
       </c>
@@ -5505,7 +5469,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>182</v>
       </c>
@@ -5513,7 +5477,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>183</v>
       </c>
@@ -5521,7 +5485,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>184</v>
       </c>
@@ -5529,7 +5493,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>52</v>
       </c>
@@ -5537,7 +5501,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>220</v>
       </c>
@@ -5545,7 +5509,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>185</v>
       </c>
@@ -5553,7 +5517,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>186</v>
       </c>
@@ -5561,7 +5525,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>187</v>
       </c>
@@ -5569,7 +5533,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>188</v>
       </c>
@@ -5577,7 +5541,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>189</v>
       </c>
@@ -5585,7 +5549,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>190</v>
       </c>
@@ -5593,7 +5557,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>191</v>
       </c>
@@ -5601,7 +5565,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>192</v>
       </c>
@@ -5609,7 +5573,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>193</v>
       </c>
@@ -5617,7 +5581,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>194</v>
       </c>
@@ -5625,7 +5589,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>53</v>
       </c>
@@ -5633,7 +5597,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>195</v>
       </c>
@@ -5641,7 +5605,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>196</v>
       </c>
@@ -5649,7 +5613,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>157</v>
       </c>
@@ -5657,7 +5621,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>197</v>
       </c>
@@ -5665,7 +5629,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>74</v>
       </c>
@@ -5673,7 +5637,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>74</v>
       </c>
@@ -5681,7 +5645,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>80</v>
       </c>
@@ -5689,7 +5653,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>51</v>
       </c>
@@ -5697,7 +5661,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>198</v>
       </c>
@@ -5705,7 +5669,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>199</v>
       </c>
@@ -5713,7 +5677,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>200</v>
       </c>
@@ -5721,7 +5685,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>201</v>
       </c>
@@ -5729,7 +5693,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>202</v>
       </c>
@@ -5737,7 +5701,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>203</v>
       </c>
@@ -5745,7 +5709,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>204</v>
       </c>
@@ -5753,7 +5717,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>50</v>
       </c>
@@ -5761,7 +5725,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>243</v>
       </c>
@@ -5769,7 +5733,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>205</v>
       </c>
@@ -5777,7 +5741,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>206</v>
       </c>
@@ -5785,7 +5749,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>207</v>
       </c>
@@ -5793,7 +5757,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>208</v>
       </c>
@@ -5801,7 +5765,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>140</v>
       </c>
@@ -5809,7 +5773,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>49</v>
       </c>
@@ -5817,7 +5781,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>237</v>
       </c>
@@ -5825,7 +5789,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>241</v>
       </c>
@@ -5833,7 +5797,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>238</v>
       </c>
@@ -5841,7 +5805,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>239</v>
       </c>
@@ -5849,7 +5813,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>240</v>
       </c>
@@ -5857,7 +5821,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>246</v>
       </c>
@@ -5865,7 +5829,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>60</v>
       </c>
@@ -5873,7 +5837,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>222</v>
       </c>
@@ -5881,7 +5845,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>218</v>
       </c>
@@ -5889,7 +5853,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>221</v>
       </c>
@@ -5897,7 +5861,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>223</v>
       </c>
@@ -5905,7 +5869,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>58</v>
       </c>
@@ -5913,7 +5877,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>26</v>
       </c>
@@ -5921,7 +5885,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>24</v>
       </c>
@@ -5929,7 +5893,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>59</v>
       </c>
@@ -5944,18 +5908,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6176,14 +6140,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B3C2A8F-D301-4EF8-A85A-44ED1557E987}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B03A569-7D12-46E7-866A-8C879B2EE202}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="6dc6a0a8-bfbb-4dfb-9ca6-66b146c89134"/>
@@ -6196,6 +6152,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B3C2A8F-D301-4EF8-A85A-44ED1557E987}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>